<commit_message>
Versión con cambio de borde
</commit_message>
<xml_diff>
--- a/Datos_pruebas/datos_deptos.xlsx
+++ b/Datos_pruebas/datos_deptos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Código Departamento</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">Número de componentes</t>
   </si>
   <si>
+    <t xml:space="preserve">Continuo</t>
+  </si>
+  <si>
     <t xml:space="preserve">NA</t>
   </si>
 </sst>
@@ -58,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,16 +143,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.68"/>
@@ -178,6 +182,9 @@
       <c r="H1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -203,6 +210,10 @@
       </c>
       <c r="H2" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>3294</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -230,6 +241,10 @@
       <c r="H3" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>3900</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -255,6 +270,10 @@
       </c>
       <c r="H4" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>4452</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,6 +301,10 @@
       <c r="H5" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>2910</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -308,6 +331,10 @@
       <c r="H6" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>3818</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -334,6 +361,10 @@
       <c r="H7" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>2555</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -360,6 +391,10 @@
       <c r="H8" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>4829</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -386,6 +421,10 @@
       <c r="H9" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>4160</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -412,6 +451,10 @@
       <c r="H10" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="I10" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>2968</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -438,6 +481,10 @@
       <c r="H11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I11" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>4317</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -464,6 +511,10 @@
       <c r="H12" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="I12" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>1530</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -490,6 +541,10 @@
       <c r="H13" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="I13" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>1105</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -516,6 +571,10 @@
       <c r="H14" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I14" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>813</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -542,6 +601,10 @@
       <c r="H15" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I15" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>1543</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -568,6 +631,10 @@
       <c r="H16" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I16" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>2113</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -594,6 +661,10 @@
       <c r="H17" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="I17" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>3228</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -620,6 +691,10 @@
       <c r="H18" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="I18" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>3635</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -646,6 +721,10 @@
       <c r="H19" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="I19" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>4465</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -672,6 +751,10 @@
       <c r="H20" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I20" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>396</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -698,6 +781,10 @@
       <c r="H21" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I21" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>2000</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -724,6 +811,10 @@
       <c r="H22" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="I22" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>3656</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -750,13 +841,17 @@
       <c r="H23" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="I23" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>268</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>0</v>
@@ -775,6 +870,10 @@
       </c>
       <c r="H24" s="0" t="n">
         <v>0</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <f aca="false">+RANDBETWEEN(1,5000)</f>
+        <v>2420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>